<commit_message>
kant FMC asset update
</commit_message>
<xml_diff>
--- a/assets uarm/2023 1 UarmPCrit/Erinias Ctonológicas.xlsx
+++ b/assets uarm/2023 1 UarmPCrit/Erinias Ctonológicas.xlsx
@@ -168,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,12 +205,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -239,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,9 +274,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -568,7 +559,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +680,7 @@
       <c r="B9" s="9">
         <v>7</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -704,7 +695,7 @@
       <c r="B10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -718,7 +709,7 @@
       <c r="B11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -734,7 +725,7 @@
       <c r="B12" s="9">
         <v>10</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3" t="s">

</xml_diff>